<commit_message>
Empresa y materia prima
</commit_message>
<xml_diff>
--- a/DB_ultimoinca.xlsx
+++ b/DB_ultimoinca.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xamppp\htdocs\Proyecto_Vino\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Proyecto_Vino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{DA1D6477-EB88-40B3-8693-58A8C1B37E94}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{800E455C-FA0A-47EE-830F-32BC45D3035B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" tabRatio="797" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" tabRatio="797" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="brix" sheetId="5" r:id="rId1"/>
@@ -51,19 +51,19 @@
     <definedName name="elultimoinca_cliente" localSheetId="4" hidden="1">Cliente!$A$1:$I$10</definedName>
     <definedName name="elultimoinca_compra_mat_pri" localSheetId="11" hidden="1">Compra_Mat_pi!$A$1:$I$2</definedName>
     <definedName name="elultimoinca_compra_venta" localSheetId="14" hidden="1">Compra_venta!$A$1:$I$2</definedName>
-    <definedName name="elultimoinca_empresa" localSheetId="8" hidden="1">Empresa!$A$1:$D$2</definedName>
+    <definedName name="elultimoinca_empresa" localSheetId="8" hidden="1">Empresa!$A$1:$D$4</definedName>
     <definedName name="elultimoinca_hoja_produccion_vino" localSheetId="17" hidden="1">Hoja_producion_vino!$A$1:$K$2</definedName>
     <definedName name="elultimoinca_hoja_producto_terminado" localSheetId="12" hidden="1">Hoja_producto_terminado!$A$1:$T$2</definedName>
     <definedName name="elultimoinca_hoja_ventas" localSheetId="21" hidden="1">Hoja_venta!$A$1:$J$2</definedName>
     <definedName name="elultimoinca_inventario_empresa" localSheetId="15" hidden="1">Inventario_empresa!$A$1:$E$2</definedName>
     <definedName name="elultimoinca_item_inventario" localSheetId="5" hidden="1">Item_inventario!$A$1:$C$6</definedName>
     <definedName name="elultimoinca_lote_1" localSheetId="24" hidden="1">Lote!$A$1:$C$2</definedName>
-    <definedName name="elultimoinca_materia_prima" localSheetId="9" hidden="1">Matria_Prima!$A$1:$D$2</definedName>
+    <definedName name="elultimoinca_materia_prima" localSheetId="9" hidden="1">Matria_Prima!$A$1:$D$15</definedName>
     <definedName name="elultimoinca_pasteurizacion" localSheetId="23" hidden="1">Pasteorizacion!$A$1:$C$2</definedName>
     <definedName name="elultimoinca_pedido" localSheetId="13" hidden="1">Pedido!$A$1:$H$2</definedName>
     <definedName name="elultimoinca_procesos" localSheetId="2" hidden="1">Proceso!$A$1:$C$3</definedName>
     <definedName name="elultimoinca_produccion_total" localSheetId="22" hidden="1">Producion_total!$A$1:$D$2</definedName>
-    <definedName name="elultimoinca_proveedor" localSheetId="10" hidden="1">Proveedor!$A$1:$G$8</definedName>
+    <definedName name="elultimoinca_proveedor" localSheetId="10" hidden="1">Proveedor!$A$1:$G$4</definedName>
     <definedName name="elultimoinca_salida_hoja_inventario" localSheetId="19" hidden="1">Salida_hoja_inventario!$A$1:$I$2</definedName>
     <definedName name="elultimoinca_socio" localSheetId="18" hidden="1">Socio!$A$1:$G$2</definedName>
     <definedName name="elultimoinca_trabajador" localSheetId="3" hidden="1">Trabajador!$A$1:$G$9</definedName>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="249">
   <si>
     <t>id</t>
   </si>
@@ -543,15 +543,6 @@
     <t>Segundo</t>
   </si>
   <si>
-    <t>05041122681</t>
-  </si>
-  <si>
-    <t>Hilda</t>
-  </si>
-  <si>
-    <t>Diaz</t>
-  </si>
-  <si>
     <t>hildadiaz85@gmail.com</t>
   </si>
   <si>
@@ -774,54 +765,18 @@
     <t>Las cajas se venderan por docenas</t>
   </si>
   <si>
-    <t xml:space="preserve">LOURDES </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> BTOAQUIZ</t>
-  </si>
-  <si>
     <t>PALLACOS</t>
   </si>
   <si>
     <t>YUNCISIG</t>
   </si>
   <si>
-    <t>05038799452</t>
-  </si>
-  <si>
-    <t>05089745621</t>
-  </si>
-  <si>
-    <t>05038792412</t>
-  </si>
-  <si>
-    <t>LORENA</t>
-  </si>
-  <si>
-    <t>MARIA</t>
-  </si>
-  <si>
-    <t>032-45867</t>
-  </si>
-  <si>
-    <t>032-48563</t>
-  </si>
-  <si>
-    <t>032-89745</t>
-  </si>
-  <si>
-    <t>032-78564</t>
-  </si>
-  <si>
     <t>lourdesBto48@hotmail.com</t>
   </si>
   <si>
     <t>lorenaPalla89@gmail.com</t>
   </si>
   <si>
-    <t>MariaYugcising78@hotmail.com</t>
-  </si>
-  <si>
     <t>gramos</t>
   </si>
   <si>
@@ -832,6 +787,126 @@
   </si>
   <si>
     <t>se muestra los gramos que se utilizo con la levadura</t>
+  </si>
+  <si>
+    <t>S/n</t>
+  </si>
+  <si>
+    <t>HIERBABUENA</t>
+  </si>
+  <si>
+    <t>S/E</t>
+  </si>
+  <si>
+    <t>QUINTICUSIG</t>
+  </si>
+  <si>
+    <t>OLGA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DIAS</t>
+  </si>
+  <si>
+    <t>S/T</t>
+  </si>
+  <si>
+    <t>s/c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOURDES  </t>
+  </si>
+  <si>
+    <t>BTOAQUIZ</t>
+  </si>
+  <si>
+    <t>id trabajador</t>
+  </si>
+  <si>
+    <t>id proveedor</t>
+  </si>
+  <si>
+    <t>id materia prima</t>
+  </si>
+  <si>
+    <t>id unidad de medida</t>
+  </si>
+  <si>
+    <t>Mortiño</t>
+  </si>
+  <si>
+    <t>Fruta silvestre</t>
+  </si>
+  <si>
+    <t>Etiqueta 750 Frente</t>
+  </si>
+  <si>
+    <t>Etiqueta 750 Detrás</t>
+  </si>
+  <si>
+    <t>Etiqueta 250 Frente</t>
+  </si>
+  <si>
+    <t>Etiqueta 250 Detrás</t>
+  </si>
+  <si>
+    <t>Corcho 750 Frente</t>
+  </si>
+  <si>
+    <t>Corcho 250 Frente</t>
+  </si>
+  <si>
+    <t>Son corchos para botellas de 750 ml</t>
+  </si>
+  <si>
+    <t>Son corechos para botellas de 250 ml</t>
+  </si>
+  <si>
+    <t>Son las etiquetas que va en la parte trasera de la botella de 250 ml</t>
+  </si>
+  <si>
+    <t>Son las etiquetas para el frente de la botellas de 250 ml</t>
+  </si>
+  <si>
+    <t>Son las etiquetas que va en la parte trasera de la botella de 750 ml</t>
+  </si>
+  <si>
+    <t>Son las etiquetas para el frente de la botellas de 750 ml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capuchon </t>
+  </si>
+  <si>
+    <t>Son los capuchones para las botellas tanto de 750 como las de 250 ml</t>
+  </si>
+  <si>
+    <t>Cinta del SRT</t>
+  </si>
+  <si>
+    <t>Son cintas del SRI para las botellas tanto de 750 como las de 250 ml</t>
+  </si>
+  <si>
+    <t>Cinta el Ultimo Inca</t>
+  </si>
+  <si>
+    <t>Es la cinta con el logo de la empresa tanto para botellas de 750 como las de 250 ml</t>
+  </si>
+  <si>
+    <t>Agua</t>
+  </si>
+  <si>
+    <t>Agua Pura</t>
+  </si>
+  <si>
+    <t>Levadura</t>
+  </si>
+  <si>
+    <t>Azucar</t>
+  </si>
+  <si>
+    <t>Levadura pura</t>
+  </si>
+  <si>
+    <t>Azucar Comun</t>
   </si>
 </sst>
 </file>
@@ -935,7 +1010,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -958,12 +1033,49 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -987,42 +1099,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1474,8 +1550,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Tabla_elultimoinca_materia_prima" displayName="Tabla_elultimoinca_materia_prima" ref="A1:D2" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D2" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Tabla_elultimoinca_materia_prima" displayName="Tabla_elultimoinca_materia_prima" ref="A1:D15" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D15" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" uniqueName="1" name="id" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" uniqueName="2" name="nombre_mat_pri" queryTableFieldId="2"/>
@@ -1487,14 +1563,14 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Tabla_elultimoinca_proveedor" displayName="Tabla_elultimoinca_proveedor" ref="A1:G8" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:G8" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Tabla_elultimoinca_proveedor" displayName="Tabla_elultimoinca_proveedor" ref="A1:G4" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:G4" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" uniqueName="1" name="id" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" uniqueName="2" name="cedula" queryTableFieldId="2" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" uniqueName="2" name="cedula" queryTableFieldId="2" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" uniqueName="3" name="nombres_pro" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" uniqueName="4" name="apellidos_pro" queryTableFieldId="4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" uniqueName="5" name="telefono_pro" queryTableFieldId="5" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" uniqueName="5" name="telefono_pro" queryTableFieldId="5" dataDxfId="10"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0A00-000006000000}" uniqueName="6" name="email_pro" queryTableFieldId="6"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0A00-000007000000}" uniqueName="7" name="id_emp" queryTableFieldId="7"/>
   </tableColumns>
@@ -1507,7 +1583,7 @@
   <autoFilter ref="A1:I2" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" uniqueName="1" name="id" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" uniqueName="2" name="fecha_mat" queryTableFieldId="2" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" uniqueName="2" name="fecha_mat" queryTableFieldId="2" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" uniqueName="3" name="precio_u_mat" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0B00-000004000000}" uniqueName="4" name="precio_tot_mat" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0B00-000005000000}" uniqueName="5" name="observaciones_mat" queryTableFieldId="5"/>
@@ -1526,11 +1602,11 @@
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" uniqueName="1" name="id" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" uniqueName="2" name="nombre" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" uniqueName="3" name="fecha" queryTableFieldId="3" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" uniqueName="3" name="fecha" queryTableFieldId="3" dataDxfId="8"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" uniqueName="4" name="valor_IVA" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" uniqueName="5" name="valor_ICE" queryTableFieldId="5"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0C00-000006000000}" uniqueName="6" name="id_paste" queryTableFieldId="6"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0C00-000007000000}" uniqueName="7" name="fecha_elb" queryTableFieldId="7" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0C00-000007000000}" uniqueName="7" name="fecha_elb" queryTableFieldId="7" dataDxfId="7"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0C00-000008000000}" uniqueName="8" name="id_lote" queryTableFieldId="8"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0C00-000009000000}" uniqueName="9" name="nombre_cantidad" queryTableFieldId="9"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0C00-00000A000000}" uniqueName="10" name="valor_cantidad" queryTableFieldId="10"/>
@@ -1554,7 +1630,7 @@
   <autoFilter ref="A1:H2" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" uniqueName="1" name="id" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" uniqueName="2" name="Fecha" queryTableFieldId="2" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" uniqueName="2" name="Fecha" queryTableFieldId="2" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0D00-000003000000}" uniqueName="3" name="unidad_medida" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0D00-000004000000}" uniqueName="4" name="Cantidad" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0D00-000005000000}" uniqueName="5" name="presentacion" queryTableFieldId="5"/>
@@ -1571,7 +1647,7 @@
   <autoFilter ref="A1:I2" xr:uid="{00000000-0009-0000-0100-00000F000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" uniqueName="1" name="id" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" uniqueName="2" name="fecha_ven" queryTableFieldId="2" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" uniqueName="2" name="fecha_ven" queryTableFieldId="2" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" uniqueName="3" name="id_tra" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0E00-000004000000}" uniqueName="4" name="Idcliente" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0E00-000005000000}" uniqueName="5" name="id_prod_total" queryTableFieldId="5"/>
@@ -1603,7 +1679,7 @@
   <autoFilter ref="A1:L2" xr:uid="{00000000-0009-0000-0100-000011000000}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" uniqueName="1" name="id" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" uniqueName="2" name="fecha_elaboracion" queryTableFieldId="2" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" uniqueName="2" name="fecha_elaboracion" queryTableFieldId="2" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1000-000003000000}" uniqueName="3" name="id_tanque" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-1000-000004000000}" uniqueName="4" name="cantidad_litros" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-1000-000005000000}" uniqueName="5" name="id_uni_medi" queryTableFieldId="5"/>
@@ -1611,7 +1687,7 @@
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-1000-000007000000}" uniqueName="7" name="id_brix" queryTableFieldId="7"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-1000-000008000000}" uniqueName="8" name="id_clase_vino" queryTableFieldId="8"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-1000-000009000000}" uniqueName="9" name="temperatura_vino" queryTableFieldId="9"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-1000-00000A000000}" uniqueName="10" name="fecha_control" queryTableFieldId="10" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-1000-00000A000000}" uniqueName="10" name="fecha_control" queryTableFieldId="10" dataDxfId="3"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-1000-00000B000000}" uniqueName="11" name="id_tra" queryTableFieldId="11"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-1000-00000C000000}" uniqueName="12" name="observaciones_area_pro" queryTableFieldId="12"/>
   </tableColumns>
@@ -1627,7 +1703,7 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" uniqueName="2" name="id_tanque" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1100-000003000000}" uniqueName="3" name="id_procesos" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-1100-000004000000}" uniqueName="4" name="id_tra" queryTableFieldId="4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1100-000005000000}" uniqueName="5" name="fecha_pro" queryTableFieldId="5" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1100-000005000000}" uniqueName="5" name="fecha_pro" queryTableFieldId="5" dataDxfId="2"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-1100-000006000000}" uniqueName="6" name="cant_fruta_klg" queryTableFieldId="6"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-1100-000007000000}" uniqueName="7" name="cant_agua_lts" queryTableFieldId="7"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-1100-000008000000}" uniqueName="8" name="cant_azucar_klg" queryTableFieldId="8"/>
@@ -1672,7 +1748,7 @@
   <autoFilter ref="A1:I2" xr:uid="{00000000-0009-0000-0100-000014000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-1300-000001000000}" uniqueName="1" name="id" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1300-000002000000}" uniqueName="2" name="fecha_sal" queryTableFieldId="2" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1300-000002000000}" uniqueName="2" name="fecha_sal" queryTableFieldId="2" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1300-000003000000}" uniqueName="3" name="saldo_sal" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-1300-000004000000}" uniqueName="4" name="ingreso_sal" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-1300-000005000000}" uniqueName="5" name="egreso_sal" queryTableFieldId="5"/>
@@ -1710,7 +1786,7 @@
   <autoFilter ref="A1:J2" xr:uid="{00000000-0009-0000-0100-000016000000}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-1500-000001000000}" uniqueName="1" name="id" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1500-000002000000}" uniqueName="2" name="fecha" queryTableFieldId="2" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1500-000002000000}" uniqueName="2" name="fecha" queryTableFieldId="2" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1500-000003000000}" uniqueName="3" name="id_tra" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-1500-000004000000}" uniqueName="4" name="id_cli" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-1500-000005000000}" uniqueName="5" name="cantidad" queryTableFieldId="5"/>
@@ -1795,7 +1871,7 @@
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" uniqueName="1" name="id" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" uniqueName="2" name="Cedula" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" uniqueName="3" name="Nombres" queryTableFieldId="3" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" uniqueName="3" name="Nombres" queryTableFieldId="3" dataDxfId="12"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" uniqueName="4" name="Apellidos" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" uniqueName="5" name="Telefono" queryTableFieldId="5"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" uniqueName="6" name="Direccion" queryTableFieldId="6"/>
@@ -1843,8 +1919,8 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tabla_elultimoinca_empresa" displayName="Tabla_elultimoinca_empresa" ref="A1:D2" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D2" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tabla_elultimoinca_empresa" displayName="Tabla_elultimoinca_empresa" ref="A1:D5" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D5" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" uniqueName="1" name="id" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" uniqueName="2" name="nombre" queryTableFieldId="2"/>
@@ -2234,17 +2310,17 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" customWidth="1"/>
+    <col min="3" max="3" width="64.140625" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2262,6 +2338,188 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>226</v>
+      </c>
+      <c r="C4" t="s">
+        <v>235</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C5" t="s">
+        <v>234</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>228</v>
+      </c>
+      <c r="C6" t="s">
+        <v>233</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>229</v>
+      </c>
+      <c r="C7" t="s">
+        <v>231</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>230</v>
+      </c>
+      <c r="C8" t="s">
+        <v>232</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>237</v>
+      </c>
+      <c r="C9" t="s">
+        <v>238</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>239</v>
+      </c>
+      <c r="C10" t="s">
+        <v>240</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>241</v>
+      </c>
+      <c r="C11" t="s">
+        <v>242</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>243</v>
+      </c>
+      <c r="C12" t="s">
+        <v>244</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>245</v>
+      </c>
+      <c r="C13" t="s">
+        <v>247</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>246</v>
+      </c>
+      <c r="C14" t="s">
+        <v>248</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2274,8 +2532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2317,19 +2575,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>130</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -2339,20 +2597,20 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>208</v>
+      <c r="B3" s="5" t="s">
+        <v>216</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="D3" t="s">
-        <v>205</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>214</v>
+        <v>218</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>215</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -2362,47 +2620,30 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C4" t="s">
         <v>209</v>
       </c>
-      <c r="C4" t="s">
-        <v>211</v>
-      </c>
       <c r="D4" t="s">
-        <v>206</v>
-      </c>
-      <c r="E4" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>215</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="G4">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="C5" t="s">
-        <v>212</v>
-      </c>
-      <c r="D5" t="s">
-        <v>207</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
+      <c r="B5" s="5"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
@@ -2418,15 +2659,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1" xr:uid="{5368A2A5-3D61-4569-A3EB-7219B471C95E}"/>
-    <hyperlink ref="F5" r:id="rId2" xr:uid="{6F6AF945-C6EB-4324-9567-EDFBA6A47122}"/>
-    <hyperlink ref="F2" r:id="rId3" xr:uid="{4AA0BD44-731B-408C-80DD-81B01E3DC353}"/>
-    <hyperlink ref="F3" r:id="rId4" xr:uid="{740AE232-EC2F-46D5-94A3-0EFD252446E2}"/>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{740AE232-EC2F-46D5-94A3-0EFD252446E2}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{4AA0BD44-731B-408C-80DD-81B01E3DC353}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{5368A2A5-3D61-4569-A3EB-7219B471C95E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2435,7 +2675,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2444,10 +2686,10 @@
     <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2481,6 +2723,18 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
+      <c r="F2" t="s">
+        <v>220</v>
+      </c>
+      <c r="G2" t="s">
+        <v>219</v>
+      </c>
+      <c r="H2" t="s">
+        <v>221</v>
+      </c>
+      <c r="I2" t="s">
+        <v>222</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2494,7 +2748,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3436,7 +3692,7 @@
         <v>113</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F2" t="s">
         <v>114</v>
@@ -3622,25 +3878,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I2">
         <v>7345</v>
@@ -3651,25 +3907,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="I3" s="9">
         <v>4587</v>
@@ -3680,25 +3936,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="I4" s="9">
         <v>9674</v>
@@ -3709,25 +3965,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="I5" s="9">
         <v>2457</v>
@@ -3738,25 +3994,25 @@
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I6" s="9">
         <v>3697</v>
@@ -3767,25 +4023,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I7" s="9">
         <v>1489</v>
@@ -3796,25 +4052,25 @@
         <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I8" s="9">
         <v>5874</v>
@@ -3825,25 +4081,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I9" s="9">
         <v>2896</v>
@@ -3854,25 +4110,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="I10" s="9">
         <v>8745</v>
@@ -3927,10 +4183,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3938,10 +4194,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C3" t="s">
         <v>197</v>
-      </c>
-      <c r="C3" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3949,10 +4205,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C4" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3960,10 +4216,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -4033,10 +4289,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -4044,10 +4300,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="C3" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -4055,10 +4311,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="C4" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -4071,14 +4327,17 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4094,6 +4353,48 @@
       </c>
       <c r="D1" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="D2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="D3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="D4" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>